<commit_message>
update flight ban (20Apr)
</commit_message>
<xml_diff>
--- a/hk-banned-inbound-flight/banned_flight_599H.xlsx
+++ b/hk-banned-inbound-flight/banned_flight_599H.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ronni\Documents\banned_flight_599h\yyipHKG.github.io\hk-banned-inbound-flight\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7FAB8E1-9B3E-417B-A623-0D98A9A82DA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4137110-100C-4F2A-97E0-3730208A074D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -975,7 +975,7 @@
   </sheetPr>
   <dimension ref="A1:L49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
       <selection activeCell="K51" sqref="K51"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
update for the week
</commit_message>
<xml_diff>
--- a/hk-banned-inbound-flight/banned_flight_599H.xlsx
+++ b/hk-banned-inbound-flight/banned_flight_599H.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ronni\Documents\banned_flight_599h\yyipHKG.github.io\hk-banned-inbound-flight\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F1458FF-C7DA-4E35-B4F4-CF6C4D9798BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B228A85D-CDE6-4E2F-90E9-01E11F00D99F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="0" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,15 +18,27 @@
   <definedNames>
     <definedName name="Z_D1F1CDC7_7748_49E3_9626_BB0A720AD03B_.wvu.FilterData" localSheetId="0" hidden="1">工作表1!$A$1:$L$26</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <customWorkbookViews>
     <customWorkbookView name="篩選器 1" guid="{D1F1CDC7-7748-49E3-9626-BB0A720AD03B}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="240">
   <si>
     <t>airline_zh</t>
   </si>
@@ -716,6 +728,36 @@
   </si>
   <si>
     <t>https://www.info.gov.hk/gia/general/202203/13/P2022031300572.htm</t>
+  </si>
+  <si>
+    <t>https://www.info.gov.hk/gia/general/202203/16/P2022031600715.htm</t>
+  </si>
+  <si>
+    <t>https://www.info.gov.hk/gia/general/202203/16/P2022031600720.htm</t>
+  </si>
+  <si>
+    <t>MH072</t>
+  </si>
+  <si>
+    <t>馬來西亞航空</t>
+  </si>
+  <si>
+    <t>Malaysia Airlines</t>
+  </si>
+  <si>
+    <t>https://www.info.gov.hk/gia/general/202203/18/P2022031800693.htm</t>
+  </si>
+  <si>
+    <t>https://www.info.gov.hk/gia/general/202203/18/P2022031800697.htm</t>
+  </si>
+  <si>
+    <t>CX702</t>
+  </si>
+  <si>
+    <t>https://www.info.gov.hk/gia/general/202203/20/P2022032000586.htm</t>
+  </si>
+  <si>
+    <t>https://www.info.gov.hk/gia/general/202203/20/P2022032000585.htm</t>
   </si>
 </sst>
 </file>
@@ -987,10 +1029,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:L55"/>
+  <dimension ref="A1:L61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="J55" sqref="J55"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="H63" sqref="H63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1059,6 +1101,7 @@
         <v>44559</v>
       </c>
       <c r="I2" s="3">
+        <f>H2+13</f>
         <v>44572</v>
       </c>
       <c r="J2" s="3">
@@ -1097,6 +1140,7 @@
         <v>44559</v>
       </c>
       <c r="I3" s="3">
+        <f t="shared" ref="I3:I61" si="0">H3+13</f>
         <v>44572</v>
       </c>
       <c r="J3" s="3">
@@ -1135,6 +1179,7 @@
         <v>44560</v>
       </c>
       <c r="I4" s="3">
+        <f t="shared" si="0"/>
         <v>44573</v>
       </c>
       <c r="J4" s="3">
@@ -1173,6 +1218,7 @@
         <v>44560</v>
       </c>
       <c r="I5" s="3">
+        <f t="shared" si="0"/>
         <v>44573</v>
       </c>
       <c r="J5" s="3">
@@ -1211,6 +1257,7 @@
         <v>44560</v>
       </c>
       <c r="I6" s="3">
+        <f t="shared" si="0"/>
         <v>44573</v>
       </c>
       <c r="J6" s="3">
@@ -1249,6 +1296,7 @@
         <v>44561</v>
       </c>
       <c r="I7" s="3">
+        <f t="shared" si="0"/>
         <v>44574</v>
       </c>
       <c r="J7" s="3">
@@ -1287,6 +1335,7 @@
         <v>44561</v>
       </c>
       <c r="I8" s="3">
+        <f t="shared" si="0"/>
         <v>44574</v>
       </c>
       <c r="J8" s="3">
@@ -1325,6 +1374,7 @@
         <v>44563</v>
       </c>
       <c r="I9" s="3">
+        <f t="shared" si="0"/>
         <v>44576</v>
       </c>
       <c r="J9" s="3">
@@ -1363,6 +1413,7 @@
         <v>44563</v>
       </c>
       <c r="I10" s="3">
+        <f t="shared" si="0"/>
         <v>44576</v>
       </c>
       <c r="J10" s="3">
@@ -1401,6 +1452,7 @@
         <v>44564</v>
       </c>
       <c r="I11" s="3">
+        <f t="shared" si="0"/>
         <v>44577</v>
       </c>
       <c r="J11" s="3">
@@ -1439,6 +1491,7 @@
         <v>44565</v>
       </c>
       <c r="I12" s="3">
+        <f t="shared" si="0"/>
         <v>44578</v>
       </c>
       <c r="J12" s="3">
@@ -1477,6 +1530,7 @@
         <v>44565</v>
       </c>
       <c r="I13" s="3">
+        <f t="shared" si="0"/>
         <v>44578</v>
       </c>
       <c r="J13" s="3">
@@ -1515,6 +1569,7 @@
         <v>44565</v>
       </c>
       <c r="I14" s="3">
+        <f t="shared" si="0"/>
         <v>44578</v>
       </c>
       <c r="J14" s="3">
@@ -1553,6 +1608,7 @@
         <v>44565</v>
       </c>
       <c r="I15" s="3">
+        <f t="shared" si="0"/>
         <v>44578</v>
       </c>
       <c r="J15" s="3">
@@ -1591,6 +1647,7 @@
         <v>44565</v>
       </c>
       <c r="I16" s="3">
+        <f t="shared" si="0"/>
         <v>44578</v>
       </c>
       <c r="J16" s="3">
@@ -1629,6 +1686,7 @@
         <v>44566</v>
       </c>
       <c r="I17" s="3">
+        <f t="shared" si="0"/>
         <v>44579</v>
       </c>
       <c r="J17" s="3">
@@ -1667,6 +1725,7 @@
         <v>44566</v>
       </c>
       <c r="I18" s="3">
+        <f t="shared" si="0"/>
         <v>44579</v>
       </c>
       <c r="J18" s="3">
@@ -1705,6 +1764,7 @@
         <v>44566</v>
       </c>
       <c r="I19" s="3">
+        <f t="shared" si="0"/>
         <v>44579</v>
       </c>
       <c r="J19" s="3">
@@ -1743,6 +1803,7 @@
         <v>44567</v>
       </c>
       <c r="I20" s="3">
+        <f t="shared" si="0"/>
         <v>44580</v>
       </c>
       <c r="J20" s="3">
@@ -1781,6 +1842,7 @@
         <v>44567</v>
       </c>
       <c r="I21" s="3">
+        <f t="shared" si="0"/>
         <v>44580</v>
       </c>
       <c r="J21" s="3">
@@ -1819,6 +1881,7 @@
         <v>44568</v>
       </c>
       <c r="I22" s="3">
+        <f t="shared" si="0"/>
         <v>44581</v>
       </c>
       <c r="J22" s="3">
@@ -1857,6 +1920,7 @@
         <v>44570</v>
       </c>
       <c r="I23" s="3">
+        <f t="shared" si="0"/>
         <v>44583</v>
       </c>
       <c r="J23" s="3">
@@ -1895,6 +1959,7 @@
         <v>44570</v>
       </c>
       <c r="I24" s="3">
+        <f t="shared" si="0"/>
         <v>44583</v>
       </c>
       <c r="J24" s="3">
@@ -1933,6 +1998,7 @@
         <v>44571</v>
       </c>
       <c r="I25" s="3">
+        <f t="shared" si="0"/>
         <v>44584</v>
       </c>
       <c r="J25" s="3">
@@ -1971,6 +2037,7 @@
         <v>44571</v>
       </c>
       <c r="I26" s="3">
+        <f t="shared" si="0"/>
         <v>44584</v>
       </c>
       <c r="J26" s="3">
@@ -2009,6 +2076,7 @@
         <v>44577</v>
       </c>
       <c r="I27" s="3">
+        <f t="shared" si="0"/>
         <v>44590</v>
       </c>
       <c r="J27" s="3">
@@ -2047,6 +2115,7 @@
         <v>44578</v>
       </c>
       <c r="I28" s="3">
+        <f t="shared" si="0"/>
         <v>44591</v>
       </c>
       <c r="J28" s="3">
@@ -2085,6 +2154,7 @@
         <v>44579</v>
       </c>
       <c r="I29" s="3">
+        <f t="shared" si="0"/>
         <v>44592</v>
       </c>
       <c r="J29" s="3">
@@ -2123,6 +2193,7 @@
         <v>44583</v>
       </c>
       <c r="I30" s="3">
+        <f t="shared" si="0"/>
         <v>44596</v>
       </c>
       <c r="J30" s="3">
@@ -2161,6 +2232,7 @@
         <v>44583</v>
       </c>
       <c r="I31" s="3">
+        <f t="shared" si="0"/>
         <v>44596</v>
       </c>
       <c r="J31" s="3">
@@ -2199,6 +2271,7 @@
         <v>44584</v>
       </c>
       <c r="I32" s="3">
+        <f t="shared" si="0"/>
         <v>44597</v>
       </c>
       <c r="J32" s="3">
@@ -2237,6 +2310,7 @@
         <v>44586</v>
       </c>
       <c r="I33" s="3">
+        <f t="shared" si="0"/>
         <v>44599</v>
       </c>
       <c r="J33" s="3">
@@ -2275,6 +2349,7 @@
         <v>44587</v>
       </c>
       <c r="I34" s="3">
+        <f t="shared" si="0"/>
         <v>44600</v>
       </c>
       <c r="J34" s="3">
@@ -2313,6 +2388,7 @@
         <v>44587</v>
       </c>
       <c r="I35" s="3">
+        <f t="shared" si="0"/>
         <v>44600</v>
       </c>
       <c r="J35" s="3">
@@ -2351,6 +2427,7 @@
         <v>44588</v>
       </c>
       <c r="I36" s="3">
+        <f t="shared" si="0"/>
         <v>44601</v>
       </c>
       <c r="J36" s="3">
@@ -2389,6 +2466,7 @@
         <v>44595</v>
       </c>
       <c r="I37" s="3">
+        <f t="shared" si="0"/>
         <v>44608</v>
       </c>
       <c r="J37" s="3">
@@ -2427,6 +2505,7 @@
         <v>44595</v>
       </c>
       <c r="I38" s="3">
+        <f t="shared" si="0"/>
         <v>44608</v>
       </c>
       <c r="J38" s="3">
@@ -2465,6 +2544,7 @@
         <v>44599</v>
       </c>
       <c r="I39" s="3">
+        <f t="shared" si="0"/>
         <v>44612</v>
       </c>
       <c r="J39" s="3">
@@ -2503,6 +2583,7 @@
         <v>44600</v>
       </c>
       <c r="I40" s="3">
+        <f t="shared" si="0"/>
         <v>44613</v>
       </c>
       <c r="J40" s="3">
@@ -2541,6 +2622,7 @@
         <v>44604</v>
       </c>
       <c r="I41" s="3">
+        <f t="shared" si="0"/>
         <v>44617</v>
       </c>
       <c r="J41" s="3">
@@ -2579,6 +2661,7 @@
         <v>44604</v>
       </c>
       <c r="I42" s="3">
+        <f t="shared" si="0"/>
         <v>44617</v>
       </c>
       <c r="J42" s="3">
@@ -2617,6 +2700,7 @@
         <v>44606</v>
       </c>
       <c r="I43" s="3">
+        <f t="shared" si="0"/>
         <v>44619</v>
       </c>
       <c r="J43" s="3">
@@ -2655,6 +2739,7 @@
         <v>44608</v>
       </c>
       <c r="I44" s="3">
+        <f t="shared" si="0"/>
         <v>44621</v>
       </c>
       <c r="J44" s="3">
@@ -2693,6 +2778,7 @@
         <v>44608</v>
       </c>
       <c r="I45" s="3">
+        <f t="shared" si="0"/>
         <v>44621</v>
       </c>
       <c r="J45" s="3">
@@ -2731,6 +2817,7 @@
         <v>44608</v>
       </c>
       <c r="I46" s="3">
+        <f t="shared" si="0"/>
         <v>44621</v>
       </c>
       <c r="J46" s="3">
@@ -2769,6 +2856,7 @@
         <v>44612</v>
       </c>
       <c r="I47" s="3">
+        <f t="shared" si="0"/>
         <v>44625</v>
       </c>
       <c r="J47" s="3">
@@ -2807,6 +2895,7 @@
         <v>44613</v>
       </c>
       <c r="I48" s="3">
+        <f t="shared" si="0"/>
         <v>44626</v>
       </c>
       <c r="J48" s="3">
@@ -2845,6 +2934,7 @@
         <v>44613</v>
       </c>
       <c r="I49" s="3">
+        <f t="shared" si="0"/>
         <v>44626</v>
       </c>
       <c r="J49" s="3">
@@ -2883,6 +2973,7 @@
         <v>44621</v>
       </c>
       <c r="I50" s="3">
+        <f t="shared" si="0"/>
         <v>44634</v>
       </c>
       <c r="J50" s="3">
@@ -2921,6 +3012,7 @@
         <v>44621</v>
       </c>
       <c r="I51" s="3">
+        <f t="shared" si="0"/>
         <v>44634</v>
       </c>
       <c r="J51" s="3">
@@ -2959,6 +3051,7 @@
         <v>44623</v>
       </c>
       <c r="I52" s="3">
+        <f t="shared" si="0"/>
         <v>44636</v>
       </c>
       <c r="J52" s="3">
@@ -2997,6 +3090,7 @@
         <v>44628</v>
       </c>
       <c r="I53" s="3">
+        <f t="shared" si="0"/>
         <v>44641</v>
       </c>
       <c r="J53" s="3">
@@ -3035,6 +3129,7 @@
         <v>44631</v>
       </c>
       <c r="I54" s="3">
+        <f t="shared" si="0"/>
         <v>44644</v>
       </c>
       <c r="J54" s="3">
@@ -3073,6 +3168,7 @@
         <v>44633</v>
       </c>
       <c r="I55" s="3">
+        <f t="shared" si="0"/>
         <v>44646</v>
       </c>
       <c r="J55" s="3">
@@ -3083,13 +3179,247 @@
       </c>
       <c r="L55" t="s">
         <v>229</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>134</v>
+      </c>
+      <c r="B56" t="s">
+        <v>135</v>
+      </c>
+      <c r="C56" t="s">
+        <v>205</v>
+      </c>
+      <c r="D56" t="s">
+        <v>208</v>
+      </c>
+      <c r="E56" t="s">
+        <v>210</v>
+      </c>
+      <c r="F56" t="s">
+        <v>208</v>
+      </c>
+      <c r="G56" t="s">
+        <v>210</v>
+      </c>
+      <c r="H56" s="3">
+        <v>44637</v>
+      </c>
+      <c r="I56" s="3">
+        <f t="shared" si="0"/>
+        <v>44650</v>
+      </c>
+      <c r="J56" s="3">
+        <v>44636</v>
+      </c>
+      <c r="K56" t="s">
+        <v>230</v>
+      </c>
+      <c r="L56" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A57" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="H57" s="3">
+        <v>44637</v>
+      </c>
+      <c r="I57" s="3">
+        <f t="shared" si="0"/>
+        <v>44650</v>
+      </c>
+      <c r="J57" s="3">
+        <v>44636</v>
+      </c>
+      <c r="K57" t="s">
+        <v>230</v>
+      </c>
+      <c r="L57" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A58" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="H58" s="3">
+        <v>44637</v>
+      </c>
+      <c r="I58" s="3">
+        <f t="shared" si="0"/>
+        <v>44650</v>
+      </c>
+      <c r="J58" s="3">
+        <v>44636</v>
+      </c>
+      <c r="K58" t="s">
+        <v>230</v>
+      </c>
+      <c r="L58" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>233</v>
+      </c>
+      <c r="B59" t="s">
+        <v>234</v>
+      </c>
+      <c r="C59" t="s">
+        <v>232</v>
+      </c>
+      <c r="D59" t="s">
+        <v>187</v>
+      </c>
+      <c r="E59" t="s">
+        <v>192</v>
+      </c>
+      <c r="F59" t="s">
+        <v>188</v>
+      </c>
+      <c r="G59" t="s">
+        <v>191</v>
+      </c>
+      <c r="H59" s="3">
+        <v>44639</v>
+      </c>
+      <c r="I59" s="3">
+        <f t="shared" si="0"/>
+        <v>44652</v>
+      </c>
+      <c r="J59" s="3">
+        <v>44638</v>
+      </c>
+      <c r="K59" t="s">
+        <v>236</v>
+      </c>
+      <c r="L59" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A60" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="H60" s="3">
+        <v>44640</v>
+      </c>
+      <c r="I60" s="3">
+        <f t="shared" si="0"/>
+        <v>44653</v>
+      </c>
+      <c r="J60" s="3">
+        <v>44640</v>
+      </c>
+      <c r="K60" t="s">
+        <v>238</v>
+      </c>
+      <c r="L60" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A61" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C61" t="s">
+        <v>237</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="H61" s="3">
+        <v>44640</v>
+      </c>
+      <c r="I61" s="3">
+        <f t="shared" si="0"/>
+        <v>44653</v>
+      </c>
+      <c r="J61" s="3">
+        <v>44640</v>
+      </c>
+      <c r="K61" t="s">
+        <v>238</v>
+      </c>
+      <c r="L61" t="s">
+        <v>239</v>
       </c>
     </row>
   </sheetData>
   <customSheetViews>
     <customSheetView guid="{D1F1CDC7-7748-49E3-9626-BB0A720AD03B}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:K26" xr:uid="{01B05965-C0EF-4E73-829F-264D73E6FB3A}"/>
+      <autoFilter ref="A1:K26" xr:uid="{3E3D086F-5BDD-4AC1-AFD2-A6A8E8F3B631}"/>
     </customSheetView>
   </customSheetViews>
   <hyperlinks>
@@ -3153,6 +3483,9 @@
     <hyperlink ref="L41" r:id="rId58" xr:uid="{8B88A62F-2025-4113-8980-6E3FA5C5C353}"/>
     <hyperlink ref="K47" r:id="rId59" xr:uid="{A5BF09DF-9B4D-4FC1-A8C2-BD090C41681A}"/>
     <hyperlink ref="L54" r:id="rId60" xr:uid="{255F47DA-2964-496D-8154-C5C1E0C5B61B}"/>
+    <hyperlink ref="L56" r:id="rId61" xr:uid="{7F288AC9-021E-4BE5-A302-A5F59E19A461}"/>
+    <hyperlink ref="L57" r:id="rId62" xr:uid="{2BC43F7F-7765-4D46-BA58-496FDB8DB281}"/>
+    <hyperlink ref="L58" r:id="rId63" xr:uid="{228D3346-EED3-42F2-A593-D94AB23467FC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
use external js, better sorting.
</commit_message>
<xml_diff>
--- a/hk-banned-inbound-flight/banned_flight_599H.xlsx
+++ b/hk-banned-inbound-flight/banned_flight_599H.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ronni\Documents\banned_flight_599h\yyipHKG.github.io\hk-banned-inbound-flight\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B1B9927-DDDE-4DF6-9A61-2F2FD2638482}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5297A06-A79F-4603-A14A-77D9012BC9F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="0" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -445,9 +445,6 @@
     <t>新加坡航空</t>
   </si>
   <si>
-    <t>Singapore Airlines</t>
-  </si>
-  <si>
     <t>SQ007</t>
   </si>
   <si>
@@ -670,9 +667,6 @@
     <t>Garuda Indonesia</t>
   </si>
   <si>
-    <t xml:space="preserve">Singapore </t>
-  </si>
-  <si>
     <t>https://www.info.gov.hk/gia/general/202202/16/P2022021600686.htm</t>
   </si>
   <si>
@@ -764,6 +758,12 @@
   </si>
   <si>
     <t>https://www.info.gov.hk/gia/general/202203/21/P2022032100575.htm</t>
+  </si>
+  <si>
+    <t>Singapore</t>
+  </si>
+  <si>
+    <t>SingaporeAirlines</t>
   </si>
 </sst>
 </file>
@@ -1037,8 +1037,8 @@
   </sheetPr>
   <dimension ref="A1:L62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="J62" sqref="J62"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1051,7 +1051,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -1072,7 +1072,7 @@
         <v>7</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>8</v>
@@ -1215,7 +1215,7 @@
         <v>37</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>38</v>
@@ -1905,10 +1905,10 @@
         <v>134</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>135</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>136</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>13</v>
@@ -1933,33 +1933,33 @@
         <v>44570</v>
       </c>
       <c r="K23" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="L23" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="L23" s="1" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="C24" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="D24" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="E24" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="F24" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="G24" s="1" t="s">
         <v>144</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>145</v>
       </c>
       <c r="H24" s="3">
         <v>44570</v>
@@ -1972,33 +1972,33 @@
         <v>44570</v>
       </c>
       <c r="K24" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="L24" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="L24" s="1" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="C25" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="D25" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="E25" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="F25" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="G25" s="1" t="s">
         <v>151</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>152</v>
       </c>
       <c r="H25" s="3">
         <v>44571</v>
@@ -2011,21 +2011,21 @@
         <v>44571</v>
       </c>
       <c r="K25" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="L25" s="1" t="s">
         <v>153</v>
-      </c>
-      <c r="L25" s="1" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="C26" s="1" t="s">
         <v>147</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>148</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>93</v>
@@ -2050,21 +2050,21 @@
         <v>44571</v>
       </c>
       <c r="K26" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="L26" s="1" t="s">
         <v>153</v>
-      </c>
-      <c r="L26" s="1" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B27" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C27" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>93</v>
@@ -2089,10 +2089,10 @@
         <v>44577</v>
       </c>
       <c r="K27" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="L27" s="1" t="s">
         <v>157</v>
-      </c>
-      <c r="L27" s="1" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
@@ -2112,7 +2112,7 @@
         <v>37</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G28" t="s">
         <v>38</v>
@@ -2128,10 +2128,10 @@
         <v>44578</v>
       </c>
       <c r="K28" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="L28" s="1" t="s">
         <v>162</v>
-      </c>
-      <c r="L28" s="1" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
@@ -2167,33 +2167,33 @@
         <v>44579</v>
       </c>
       <c r="K29" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="L29" s="1" t="s">
         <v>165</v>
-      </c>
-      <c r="L29" s="1" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
+        <v>166</v>
+      </c>
+      <c r="B30" t="s">
+        <v>170</v>
+      </c>
+      <c r="C30" t="s">
         <v>167</v>
       </c>
-      <c r="B30" t="s">
+      <c r="D30" t="s">
+        <v>168</v>
+      </c>
+      <c r="E30" t="s">
         <v>171</v>
       </c>
-      <c r="C30" t="s">
-        <v>168</v>
-      </c>
-      <c r="D30" t="s">
-        <v>169</v>
-      </c>
-      <c r="E30" t="s">
+      <c r="F30" t="s">
+        <v>173</v>
+      </c>
+      <c r="G30" t="s">
         <v>172</v>
-      </c>
-      <c r="F30" t="s">
-        <v>174</v>
-      </c>
-      <c r="G30" t="s">
-        <v>173</v>
       </c>
       <c r="H30" s="3">
         <v>44583</v>
@@ -2206,21 +2206,21 @@
         <v>44583</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
+        <v>166</v>
+      </c>
+      <c r="B31" t="s">
+        <v>170</v>
+      </c>
+      <c r="C31" t="s">
         <v>167</v>
-      </c>
-      <c r="B31" t="s">
-        <v>171</v>
-      </c>
-      <c r="C31" t="s">
-        <v>168</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>93</v>
@@ -2245,10 +2245,10 @@
         <v>44583</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
@@ -2284,10 +2284,10 @@
         <v>44584</v>
       </c>
       <c r="K32" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="L32" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="L32" s="1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
@@ -2323,33 +2323,33 @@
         <v>44586</v>
       </c>
       <c r="K33" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="L33" s="1" t="s">
         <v>178</v>
-      </c>
-      <c r="L33" s="1" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="C34" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="D34" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="E34" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="F34" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="F34" s="1" t="s">
+      <c r="G34" s="1" t="s">
         <v>151</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>152</v>
       </c>
       <c r="H34" s="3">
         <v>44587</v>
@@ -2362,21 +2362,21 @@
         <v>44587</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="L34" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="C35" s="1" t="s">
         <v>147</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>148</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>93</v>
@@ -2401,10 +2401,10 @@
         <v>44587</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="L35" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="36" spans="1:12" ht="15" x14ac:dyDescent="0.25">
@@ -2440,10 +2440,10 @@
         <v>44588</v>
       </c>
       <c r="K36" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="L36" s="1" t="s">
         <v>182</v>
-      </c>
-      <c r="L36" s="1" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
@@ -2463,7 +2463,7 @@
         <v>37</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G37" t="s">
         <v>38</v>
@@ -2479,10 +2479,10 @@
         <v>44595</v>
       </c>
       <c r="K37" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="L37" s="1" t="s">
         <v>184</v>
-      </c>
-      <c r="L37" s="1" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
@@ -2518,10 +2518,10 @@
         <v>44595</v>
       </c>
       <c r="K38" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="L38" s="1" t="s">
         <v>184</v>
-      </c>
-      <c r="L38" s="1" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.2">
@@ -2532,19 +2532,19 @@
         <v>11</v>
       </c>
       <c r="C39" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="D39" t="s">
         <v>186</v>
       </c>
-      <c r="D39" t="s">
+      <c r="E39" t="s">
+        <v>191</v>
+      </c>
+      <c r="F39" t="s">
         <v>187</v>
       </c>
-      <c r="E39" t="s">
-        <v>192</v>
-      </c>
-      <c r="F39" t="s">
-        <v>188</v>
-      </c>
       <c r="G39" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H39" s="3">
         <v>44599</v>
@@ -2557,10 +2557,10 @@
         <v>44599</v>
       </c>
       <c r="K39" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="L39" s="1" t="s">
         <v>189</v>
-      </c>
-      <c r="L39" s="1" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.2">
@@ -2596,33 +2596,33 @@
         <v>44600</v>
       </c>
       <c r="K40" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="L40" s="1" t="s">
         <v>193</v>
-      </c>
-      <c r="L40" s="1" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="C41" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="D41" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="D41" s="1" t="s">
+      <c r="E41" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="E41" s="1" t="s">
+      <c r="F41" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="F41" s="1" t="s">
+      <c r="G41" s="1" t="s">
         <v>151</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>152</v>
       </c>
       <c r="H41" s="3">
         <v>44604</v>
@@ -2635,21 +2635,21 @@
         <v>44604</v>
       </c>
       <c r="K41" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="L41" s="1" t="s">
         <v>153</v>
-      </c>
-      <c r="L41" s="1" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="C42" s="1" t="s">
         <v>147</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>148</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>93</v>
@@ -2674,10 +2674,10 @@
         <v>44604</v>
       </c>
       <c r="K42" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="L42" s="1" t="s">
         <v>195</v>
-      </c>
-      <c r="L42" s="1" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.2">
@@ -2688,19 +2688,19 @@
         <v>11</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D43" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="F43" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="E43" s="1" t="s">
+      <c r="G43" s="1" t="s">
         <v>201</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="G43" s="1" t="s">
-        <v>202</v>
       </c>
       <c r="H43" s="3">
         <v>44606</v>
@@ -2713,10 +2713,10 @@
         <v>44606</v>
       </c>
       <c r="K43" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="L43" s="1" t="s">
         <v>199</v>
-      </c>
-      <c r="L43" s="1" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.2">
@@ -2724,22 +2724,22 @@
         <v>134</v>
       </c>
       <c r="B44" t="s">
-        <v>135</v>
+        <v>241</v>
       </c>
       <c r="C44" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D44" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E44" t="s">
-        <v>210</v>
+        <v>240</v>
       </c>
       <c r="F44" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G44" t="s">
-        <v>210</v>
+        <v>240</v>
       </c>
       <c r="H44" s="3">
         <v>44608</v>
@@ -2752,10 +2752,10 @@
         <v>44608</v>
       </c>
       <c r="K44" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="L44" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.2">
@@ -2763,22 +2763,22 @@
         <v>134</v>
       </c>
       <c r="B45" t="s">
-        <v>135</v>
+        <v>241</v>
       </c>
       <c r="C45" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D45" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E45" t="s">
-        <v>210</v>
+        <v>240</v>
       </c>
       <c r="F45" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G45" t="s">
-        <v>210</v>
+        <v>240</v>
       </c>
       <c r="H45" s="3">
         <v>44608</v>
@@ -2791,33 +2791,33 @@
         <v>44608</v>
       </c>
       <c r="K45" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="L45" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B46" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C46" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D46" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="F46" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="E46" s="1" t="s">
+      <c r="G46" s="1" t="s">
         <v>201</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="G46" s="1" t="s">
-        <v>202</v>
       </c>
       <c r="H46" s="3">
         <v>44608</v>
@@ -2830,10 +2830,10 @@
         <v>44608</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="L46" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.2">
@@ -2869,10 +2869,10 @@
         <v>44612</v>
       </c>
       <c r="K47" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="L47" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.2">
@@ -2908,33 +2908,33 @@
         <v>44613</v>
       </c>
       <c r="K48" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="L48" s="1" t="s">
         <v>217</v>
-      </c>
-      <c r="L48" s="1" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
+        <v>214</v>
+      </c>
+      <c r="B49" t="s">
         <v>216</v>
       </c>
-      <c r="B49" t="s">
-        <v>218</v>
-      </c>
       <c r="C49" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D49" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E49" t="s">
-        <v>210</v>
+        <v>240</v>
       </c>
       <c r="F49" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G49" t="s">
-        <v>210</v>
+        <v>240</v>
       </c>
       <c r="H49" s="3">
         <v>44613</v>
@@ -2947,33 +2947,33 @@
         <v>44613</v>
       </c>
       <c r="K49" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="L49" s="1" t="s">
         <v>217</v>
-      </c>
-      <c r="L49" s="1" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B50" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="C50" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="D50" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="D50" s="1" t="s">
+      <c r="E50" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="E50" s="1" t="s">
+      <c r="F50" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="F50" s="1" t="s">
+      <c r="G50" s="1" t="s">
         <v>151</v>
-      </c>
-      <c r="G50" s="1" t="s">
-        <v>152</v>
       </c>
       <c r="H50" s="3">
         <v>44621</v>
@@ -2986,21 +2986,21 @@
         <v>44621</v>
       </c>
       <c r="K50" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="L50" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B51" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="C51" s="1" t="s">
         <v>147</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>148</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>93</v>
@@ -3025,10 +3025,10 @@
         <v>44621</v>
       </c>
       <c r="K51" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="L51" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.2">
@@ -3039,19 +3039,19 @@
         <v>11</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D52" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="F52" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="E52" s="1" t="s">
+      <c r="G52" s="1" t="s">
         <v>201</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="G52" s="1" t="s">
-        <v>202</v>
       </c>
       <c r="H52" s="3">
         <v>44623</v>
@@ -3064,33 +3064,33 @@
         <v>44622</v>
       </c>
       <c r="K52" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="L52" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B53" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C53" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D53" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="F53" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="E53" s="1" t="s">
+      <c r="G53" s="1" t="s">
         <v>201</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="G53" s="1" t="s">
-        <v>202</v>
       </c>
       <c r="H53" s="3">
         <v>44628</v>
@@ -3103,10 +3103,10 @@
         <v>44627</v>
       </c>
       <c r="K53" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="L53" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.2">
@@ -3142,10 +3142,10 @@
         <v>44631</v>
       </c>
       <c r="K54" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="L54" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.2">
@@ -3181,10 +3181,10 @@
         <v>44633</v>
       </c>
       <c r="K55" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="L55" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.2">
@@ -3192,22 +3192,22 @@
         <v>134</v>
       </c>
       <c r="B56" t="s">
-        <v>135</v>
+        <v>241</v>
       </c>
       <c r="C56" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D56" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E56" t="s">
-        <v>210</v>
+        <v>240</v>
       </c>
       <c r="F56" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G56" t="s">
-        <v>210</v>
+        <v>240</v>
       </c>
       <c r="H56" s="3">
         <v>44637</v>
@@ -3220,33 +3220,33 @@
         <v>44636</v>
       </c>
       <c r="K56" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="L56" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B57" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="C57" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="C57" s="1" t="s">
+      <c r="D57" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="D57" s="1" t="s">
+      <c r="E57" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="E57" s="1" t="s">
+      <c r="F57" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="F57" s="1" t="s">
+      <c r="G57" s="1" t="s">
         <v>151</v>
-      </c>
-      <c r="G57" s="1" t="s">
-        <v>152</v>
       </c>
       <c r="H57" s="3">
         <v>44637</v>
@@ -3259,21 +3259,21 @@
         <v>44636</v>
       </c>
       <c r="K57" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="L57" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B58" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="C58" s="1" t="s">
         <v>147</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>148</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>93</v>
@@ -3298,33 +3298,33 @@
         <v>44636</v>
       </c>
       <c r="K58" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="L58" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B59" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C59" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D59" t="s">
+        <v>186</v>
+      </c>
+      <c r="E59" t="s">
+        <v>191</v>
+      </c>
+      <c r="F59" t="s">
         <v>187</v>
       </c>
-      <c r="E59" t="s">
-        <v>192</v>
-      </c>
-      <c r="F59" t="s">
-        <v>188</v>
-      </c>
       <c r="G59" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H59" s="3">
         <v>44639</v>
@@ -3337,10 +3337,10 @@
         <v>44638</v>
       </c>
       <c r="K59" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="L59" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.2">
@@ -3351,19 +3351,19 @@
         <v>11</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D60" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="F60" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="E60" s="1" t="s">
+      <c r="G60" s="1" t="s">
         <v>201</v>
-      </c>
-      <c r="F60" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="G60" s="1" t="s">
-        <v>202</v>
       </c>
       <c r="H60" s="3">
         <v>44640</v>
@@ -3376,10 +3376,10 @@
         <v>44640</v>
       </c>
       <c r="K60" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="L60" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.2">
@@ -3390,7 +3390,7 @@
         <v>11</v>
       </c>
       <c r="C61" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>93</v>
@@ -3415,10 +3415,10 @@
         <v>44640</v>
       </c>
       <c r="K61" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="L61" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.2">
@@ -3438,7 +3438,7 @@
         <v>37</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G62" t="s">
         <v>38</v>
@@ -3454,17 +3454,17 @@
         <v>44641</v>
       </c>
       <c r="K62" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="L62" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
   </sheetData>
   <customSheetViews>
     <customSheetView guid="{D1F1CDC7-7748-49E3-9626-BB0A720AD03B}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:K26" xr:uid="{843EB117-01FE-4995-9C92-DFFEA3E12A1C}"/>
+      <autoFilter ref="A1:K26" xr:uid="{E304C89A-0D9E-4389-98D8-D87CDA569ADB}"/>
     </customSheetView>
   </customSheetViews>
   <hyperlinks>

</xml_diff>